<commit_message>
Time to submit, data-analysis
</commit_message>
<xml_diff>
--- a/Model2/excel/DemR/PriceProf.xlsx
+++ b/Model2/excel/DemR/PriceProf.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7590" tabRatio="681" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7590" tabRatio="681" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Winter-wd" sheetId="3" r:id="rId1"/>
@@ -354,7 +354,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,76 +438,76 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>55.5</v>
+        <v>48.944624780929573</v>
       </c>
       <c r="C2">
-        <v>55.5</v>
+        <v>43.622658697783599</v>
       </c>
       <c r="D2">
-        <v>55.5</v>
+        <v>39.785869761391325</v>
       </c>
       <c r="E2">
-        <v>55.5</v>
+        <v>35.339140722213898</v>
       </c>
       <c r="F2">
-        <v>55.5</v>
+        <v>34.399946907223317</v>
       </c>
       <c r="G2">
-        <v>55.5</v>
+        <v>38.497734686852816</v>
       </c>
       <c r="H2">
-        <v>55.5</v>
+        <v>46.68209985724301</v>
       </c>
       <c r="I2">
-        <v>55.5</v>
+        <v>56.86108389365085</v>
       </c>
       <c r="J2">
-        <v>55.5</v>
+        <v>61.509879300107698</v>
       </c>
       <c r="K2">
-        <v>55.5</v>
+        <v>64.005432747320356</v>
       </c>
       <c r="L2">
-        <v>55.5</v>
+        <v>64.479988390425845</v>
       </c>
       <c r="M2">
-        <v>55.5</v>
+        <v>65.1025028684668</v>
       </c>
       <c r="N2">
-        <v>55.5</v>
+        <v>63.0149505850612</v>
       </c>
       <c r="O2">
-        <v>55.5</v>
+        <v>59.302777027107354</v>
       </c>
       <c r="P2">
-        <v>55.5</v>
+        <v>56.521452036326195</v>
       </c>
       <c r="Q2">
-        <v>55.5</v>
+        <v>53.889464876308658</v>
       </c>
       <c r="R2">
-        <v>55.5</v>
+        <v>53.659291613963418</v>
       </c>
       <c r="S2">
-        <v>55.5</v>
+        <v>61.521851209167799</v>
       </c>
       <c r="T2">
-        <v>55.5</v>
+        <v>68.095062982422306</v>
       </c>
       <c r="U2">
-        <v>55.5</v>
+        <v>68.305684417863745</v>
       </c>
       <c r="V2">
-        <v>55.5</v>
+        <v>62.993558244454753</v>
       </c>
       <c r="W2">
-        <v>55.5</v>
+        <v>58.1847630441682</v>
       </c>
       <c r="X2">
-        <v>55.5</v>
+        <v>60.070880904817756</v>
       </c>
       <c r="Y2">
-        <v>55.5</v>
+        <v>55.209300444730303</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +520,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,76 +604,76 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>55.6</v>
+        <v>48.944624780929573</v>
       </c>
       <c r="C2">
-        <v>55.6</v>
+        <v>43.622658697783599</v>
       </c>
       <c r="D2">
-        <v>55.6</v>
+        <v>39.785869761391325</v>
       </c>
       <c r="E2">
-        <v>55.6</v>
+        <v>35.339140722213898</v>
       </c>
       <c r="F2">
-        <v>55.6</v>
+        <v>34.399946907223317</v>
       </c>
       <c r="G2">
-        <v>55.6</v>
+        <v>38.497734686852816</v>
       </c>
       <c r="H2">
-        <v>55.6</v>
+        <v>46.68209985724301</v>
       </c>
       <c r="I2">
-        <v>55.6</v>
+        <v>56.86108389365085</v>
       </c>
       <c r="J2">
-        <v>55.6</v>
+        <v>61.509879300107698</v>
       </c>
       <c r="K2">
-        <v>55.6</v>
+        <v>64.005432747320356</v>
       </c>
       <c r="L2">
-        <v>55.6</v>
+        <v>64.479988390425845</v>
       </c>
       <c r="M2">
-        <v>55.6</v>
+        <v>65.1025028684668</v>
       </c>
       <c r="N2">
-        <v>55.6</v>
+        <v>63.0149505850612</v>
       </c>
       <c r="O2">
-        <v>55.6</v>
+        <v>59.302777027107354</v>
       </c>
       <c r="P2">
-        <v>55.6</v>
+        <v>56.521452036326195</v>
       </c>
       <c r="Q2">
-        <v>55.6</v>
+        <v>53.889464876308658</v>
       </c>
       <c r="R2">
-        <v>55.6</v>
+        <v>53.659291613963418</v>
       </c>
       <c r="S2">
-        <v>55.6</v>
+        <v>61.521851209167799</v>
       </c>
       <c r="T2">
-        <v>55.6</v>
+        <v>68.095062982422306</v>
       </c>
       <c r="U2">
-        <v>55.6</v>
+        <v>68.305684417863745</v>
       </c>
       <c r="V2">
-        <v>55.6</v>
+        <v>62.993558244454753</v>
       </c>
       <c r="W2">
-        <v>55.6</v>
+        <v>58.1847630441682</v>
       </c>
       <c r="X2">
-        <v>55.6</v>
+        <v>60.070880904817756</v>
       </c>
       <c r="Y2">
-        <v>55.6</v>
+        <v>55.209300444730303</v>
       </c>
     </row>
   </sheetData>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1166,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,76 +1250,76 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>55.5</v>
+        <v>48.944624780929573</v>
       </c>
       <c r="C2">
-        <v>55.5</v>
+        <v>43.622658697783599</v>
       </c>
       <c r="D2">
-        <v>55.5</v>
+        <v>39.785869761391325</v>
       </c>
       <c r="E2">
-        <v>55.5</v>
+        <v>35.339140722213898</v>
       </c>
       <c r="F2">
-        <v>55.5</v>
+        <v>34.399946907223317</v>
       </c>
       <c r="G2">
-        <v>55.5</v>
+        <v>38.497734686852816</v>
       </c>
       <c r="H2">
-        <v>55.5</v>
+        <v>46.68209985724301</v>
       </c>
       <c r="I2">
-        <v>55.5</v>
+        <v>56.86108389365085</v>
       </c>
       <c r="J2">
-        <v>55.5</v>
+        <v>61.509879300107698</v>
       </c>
       <c r="K2">
-        <v>55.5</v>
+        <v>64.005432747320356</v>
       </c>
       <c r="L2">
-        <v>55.5</v>
+        <v>64.479988390425845</v>
       </c>
       <c r="M2">
-        <v>55.5</v>
+        <v>65.1025028684668</v>
       </c>
       <c r="N2">
-        <v>55.5</v>
+        <v>63.0149505850612</v>
       </c>
       <c r="O2">
-        <v>55.5</v>
+        <v>59.302777027107354</v>
       </c>
       <c r="P2">
-        <v>55.5</v>
+        <v>56.521452036326195</v>
       </c>
       <c r="Q2">
-        <v>55.5</v>
+        <v>53.889464876308658</v>
       </c>
       <c r="R2">
-        <v>55.5</v>
+        <v>53.659291613963418</v>
       </c>
       <c r="S2">
-        <v>55.5</v>
+        <v>61.521851209167799</v>
       </c>
       <c r="T2">
-        <v>55.5</v>
+        <v>68.095062982422306</v>
       </c>
       <c r="U2">
-        <v>55.5</v>
+        <v>68.305684417863745</v>
       </c>
       <c r="V2">
-        <v>55.5</v>
+        <v>62.993558244454753</v>
       </c>
       <c r="W2">
-        <v>55.5</v>
+        <v>58.1847630441682</v>
       </c>
       <c r="X2">
-        <v>55.5</v>
+        <v>60.070880904817756</v>
       </c>
       <c r="Y2">
-        <v>55.5</v>
+        <v>55.209300444730303</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,76 +1416,76 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>55.6</v>
+        <v>48.944624780929573</v>
       </c>
       <c r="C2">
-        <v>55.6</v>
+        <v>43.622658697783599</v>
       </c>
       <c r="D2">
-        <v>55.6</v>
+        <v>39.785869761391325</v>
       </c>
       <c r="E2">
-        <v>55.6</v>
+        <v>35.339140722213898</v>
       </c>
       <c r="F2">
-        <v>55.6</v>
+        <v>34.399946907223317</v>
       </c>
       <c r="G2">
-        <v>55.6</v>
+        <v>38.497734686852816</v>
       </c>
       <c r="H2">
-        <v>55.6</v>
+        <v>46.68209985724301</v>
       </c>
       <c r="I2">
-        <v>55.6</v>
+        <v>56.86108389365085</v>
       </c>
       <c r="J2">
-        <v>55.6</v>
+        <v>61.509879300107698</v>
       </c>
       <c r="K2">
-        <v>55.6</v>
+        <v>64.005432747320356</v>
       </c>
       <c r="L2">
-        <v>55.6</v>
+        <v>64.479988390425845</v>
       </c>
       <c r="M2">
-        <v>55.6</v>
+        <v>65.1025028684668</v>
       </c>
       <c r="N2">
-        <v>55.6</v>
+        <v>63.0149505850612</v>
       </c>
       <c r="O2">
-        <v>55.6</v>
+        <v>59.302777027107354</v>
       </c>
       <c r="P2">
-        <v>55.6</v>
+        <v>56.521452036326195</v>
       </c>
       <c r="Q2">
-        <v>55.6</v>
+        <v>53.889464876308658</v>
       </c>
       <c r="R2">
-        <v>55.6</v>
+        <v>53.659291613963418</v>
       </c>
       <c r="S2">
-        <v>55.6</v>
+        <v>61.521851209167799</v>
       </c>
       <c r="T2">
-        <v>55.6</v>
+        <v>68.095062982422306</v>
       </c>
       <c r="U2">
-        <v>55.6</v>
+        <v>68.305684417863745</v>
       </c>
       <c r="V2">
-        <v>55.6</v>
+        <v>62.993558244454753</v>
       </c>
       <c r="W2">
-        <v>55.6</v>
+        <v>58.1847630441682</v>
       </c>
       <c r="X2">
-        <v>55.6</v>
+        <v>60.070880904817756</v>
       </c>
       <c r="Y2">
-        <v>55.6</v>
+        <v>55.209300444730303</v>
       </c>
     </row>
   </sheetData>
@@ -1498,7 +1498,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,76 +1582,76 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>55.5</v>
+        <v>48.944624780929573</v>
       </c>
       <c r="C2">
-        <v>55.5</v>
+        <v>43.622658697783599</v>
       </c>
       <c r="D2">
-        <v>55.5</v>
+        <v>39.785869761391325</v>
       </c>
       <c r="E2">
-        <v>55.5</v>
+        <v>35.339140722213898</v>
       </c>
       <c r="F2">
-        <v>55.5</v>
+        <v>34.399946907223317</v>
       </c>
       <c r="G2">
-        <v>55.5</v>
+        <v>38.497734686852816</v>
       </c>
       <c r="H2">
-        <v>55.5</v>
+        <v>46.68209985724301</v>
       </c>
       <c r="I2">
-        <v>55.5</v>
+        <v>56.86108389365085</v>
       </c>
       <c r="J2">
-        <v>55.5</v>
+        <v>61.509879300107698</v>
       </c>
       <c r="K2">
-        <v>55.5</v>
+        <v>64.005432747320356</v>
       </c>
       <c r="L2">
-        <v>55.5</v>
+        <v>64.479988390425845</v>
       </c>
       <c r="M2">
-        <v>55.5</v>
+        <v>65.1025028684668</v>
       </c>
       <c r="N2">
-        <v>55.5</v>
+        <v>63.0149505850612</v>
       </c>
       <c r="O2">
-        <v>55.5</v>
+        <v>59.302777027107354</v>
       </c>
       <c r="P2">
-        <v>55.5</v>
+        <v>56.521452036326195</v>
       </c>
       <c r="Q2">
-        <v>55.5</v>
+        <v>53.889464876308658</v>
       </c>
       <c r="R2">
-        <v>55.5</v>
+        <v>53.659291613963418</v>
       </c>
       <c r="S2">
-        <v>55.5</v>
+        <v>61.521851209167799</v>
       </c>
       <c r="T2">
-        <v>55.5</v>
+        <v>68.095062982422306</v>
       </c>
       <c r="U2">
-        <v>55.5</v>
+        <v>68.305684417863745</v>
       </c>
       <c r="V2">
-        <v>55.5</v>
+        <v>62.993558244454753</v>
       </c>
       <c r="W2">
-        <v>55.5</v>
+        <v>58.1847630441682</v>
       </c>
       <c r="X2">
-        <v>55.5</v>
+        <v>60.070880904817756</v>
       </c>
       <c r="Y2">
-        <v>55.5</v>
+        <v>55.209300444730303</v>
       </c>
     </row>
   </sheetData>
@@ -1663,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,76 +1748,76 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>55.6</v>
+        <v>48.944624780929573</v>
       </c>
       <c r="C2">
-        <v>55.6</v>
+        <v>43.622658697783599</v>
       </c>
       <c r="D2">
-        <v>55.6</v>
+        <v>39.785869761391325</v>
       </c>
       <c r="E2">
-        <v>55.6</v>
+        <v>35.339140722213898</v>
       </c>
       <c r="F2">
-        <v>55.6</v>
+        <v>34.399946907223317</v>
       </c>
       <c r="G2">
-        <v>55.6</v>
+        <v>38.497734686852816</v>
       </c>
       <c r="H2">
-        <v>55.6</v>
+        <v>46.68209985724301</v>
       </c>
       <c r="I2">
-        <v>55.6</v>
+        <v>56.86108389365085</v>
       </c>
       <c r="J2">
-        <v>55.6</v>
+        <v>61.509879300107698</v>
       </c>
       <c r="K2">
-        <v>55.6</v>
+        <v>64.005432747320356</v>
       </c>
       <c r="L2">
-        <v>55.6</v>
+        <v>64.479988390425845</v>
       </c>
       <c r="M2">
-        <v>55.6</v>
+        <v>65.1025028684668</v>
       </c>
       <c r="N2">
-        <v>55.6</v>
+        <v>63.0149505850612</v>
       </c>
       <c r="O2">
-        <v>55.6</v>
+        <v>59.302777027107354</v>
       </c>
       <c r="P2">
-        <v>55.6</v>
+        <v>56.521452036326195</v>
       </c>
       <c r="Q2">
-        <v>55.6</v>
+        <v>53.889464876308658</v>
       </c>
       <c r="R2">
-        <v>55.6</v>
+        <v>53.659291613963418</v>
       </c>
       <c r="S2">
-        <v>55.6</v>
+        <v>61.521851209167799</v>
       </c>
       <c r="T2">
-        <v>55.6</v>
+        <v>68.095062982422306</v>
       </c>
       <c r="U2">
-        <v>55.6</v>
+        <v>68.305684417863745</v>
       </c>
       <c r="V2">
-        <v>55.6</v>
+        <v>62.993558244454753</v>
       </c>
       <c r="W2">
-        <v>55.6</v>
+        <v>58.1847630441682</v>
       </c>
       <c r="X2">
-        <v>55.6</v>
+        <v>60.070880904817756</v>
       </c>
       <c r="Y2">
-        <v>55.6</v>
+        <v>55.209300444730303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>